<commit_message>
Can view roster on user page
</commit_message>
<xml_diff>
--- a/app/data/champions.xlsx
+++ b/app/data/champions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="125">
   <si>
     <t>Soraka</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>Tank</t>
+  </si>
+  <si>
+    <t>Vi</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="L114" sqref="L114"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,34 +736,34 @@
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,255)</f>
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="C1">
         <f t="shared" ref="C1:F17" ca="1" si="0">RANDBETWEEN(1,255)</f>
-        <v>79</v>
+        <v>184</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="F1">
         <f ca="1">RANDBETWEEN(1,255)</f>
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1">
         <f ca="1">RANDBETWEEN(1,7800)</f>
-        <v>7070</v>
+        <v>1066</v>
       </c>
       <c r="I1">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -769,34 +772,34 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B65" ca="1" si="1">RANDBETWEEN(1,255)</f>
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>240</v>
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,255)</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>119</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H65" ca="1" si="2">RANDBETWEEN(1,7800)</f>
-        <v>6455</v>
+        <v>3488</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I65" ca="1" si="3">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -805,34 +808,34 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>208</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>204</v>
+        <v>167</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>164</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(1,255)</f>
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="G3" t="s">
         <v>120</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="2"/>
-        <v>5099</v>
+        <v>714</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,34 +844,34 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>198</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(1,255)</f>
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="G4" t="s">
         <v>121</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
-        <v>7720</v>
+        <v>832</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -877,30 +880,30 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>248</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>249</v>
+        <v>87</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
         <v>122</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
-        <v>5261</v>
+        <v>2068</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
@@ -913,34 +916,34 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>241</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>219</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>168</v>
       </c>
       <c r="G6" t="s">
         <v>123</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>2145</v>
+        <v>6865</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -949,34 +952,34 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>214</v>
+        <v>126</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>206</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>219</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
-        <v>5233</v>
+        <v>7036</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -985,34 +988,34 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>212</v>
+        <v>120</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>243</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="G8" t="s">
         <v>119</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>7131</v>
+        <v>7106</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,34 +1024,34 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>246</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>191</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>239</v>
+        <v>175</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
         <v>120</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>2467</v>
+        <v>5895</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,34 +1060,34 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>238</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="G10" t="s">
         <v>121</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>2386</v>
+        <v>4930</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1093,34 +1096,34 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>137</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>44</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
         <v>122</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>2953</v>
+        <v>6502</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,19 +1132,19 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>244</v>
+        <v>119</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>235</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
@@ -1152,11 +1155,11 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>7003</v>
+        <v>3382</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1165,34 +1168,34 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
         <v>1</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>348</v>
+        <v>3362</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1201,34 +1204,34 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>238</v>
+        <v>120</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="G14" t="s">
         <v>119</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>7080</v>
+        <v>6346</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,34 +1240,34 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>253</v>
+        <v>104</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>244</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>120</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>5295</v>
+        <v>3295</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1273,34 +1276,34 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>225</v>
+        <v>77</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G16" t="s">
         <v>121</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
-        <v>4312</v>
+        <v>6853</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,34 +1312,34 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:C80" ca="1" si="4">RANDBETWEEN(1,255)</f>
-        <v>12</v>
+        <v>158</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:D80" ca="1" si="5">RANDBETWEEN(1,255)</f>
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="E17">
         <f t="shared" ref="E17:E80" ca="1" si="6">RANDBETWEEN(1,255)</f>
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
         <v>122</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>5646</v>
+        <v>1060</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,34 +1348,34 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>157</v>
+        <v>243</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="4"/>
-        <v>134</v>
+        <v>220</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="5"/>
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="6"/>
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F81" ca="1" si="7">RANDBETWEEN(1,255)</f>
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="G18" t="s">
         <v>123</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>1376</v>
+        <v>3808</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1381,34 +1384,34 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>238</v>
+        <v>70</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="4"/>
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="7"/>
-        <v>132</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
         <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>809</v>
+        <v>1925</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1417,34 +1420,34 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>208</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="4"/>
-        <v>114</v>
+        <v>208</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="5"/>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="6"/>
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="7"/>
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
         <v>119</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>7609</v>
+        <v>840</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1453,30 +1456,30 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="6"/>
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="7"/>
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="G21" t="s">
         <v>120</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>4199</v>
+        <v>3490</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="3"/>
@@ -1489,34 +1492,34 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="4"/>
-        <v>135</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="6"/>
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="7"/>
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
         <v>121</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1823</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1525,34 +1528,34 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="4"/>
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="5"/>
-        <v>171</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="6"/>
-        <v>101</v>
+        <v>245</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="7"/>
-        <v>239</v>
+        <v>68</v>
       </c>
       <c r="G23" t="s">
         <v>122</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>1197</v>
+        <v>6603</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1561,34 +1564,34 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="4"/>
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="5"/>
-        <v>242</v>
+        <v>72</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="6"/>
-        <v>210</v>
+        <v>65</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="7"/>
-        <v>209</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
         <v>123</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>5313</v>
+        <v>1297</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,34 +1600,34 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>215</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="5"/>
         <v>183</v>
       </c>
-      <c r="D25">
-        <f t="shared" ca="1" si="5"/>
-        <v>192</v>
-      </c>
       <c r="E25">
         <f t="shared" ca="1" si="6"/>
-        <v>152</v>
+        <v>3</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="7"/>
-        <v>244</v>
+        <v>64</v>
       </c>
       <c r="G25" t="s">
         <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>6765</v>
+        <v>5011</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1633,34 +1636,34 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="4"/>
-        <v>221</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="5"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="6"/>
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="7"/>
-        <v>112</v>
+        <v>254</v>
       </c>
       <c r="G26" t="s">
         <v>119</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>7004</v>
+        <v>131</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1669,34 +1672,34 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>198</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="4"/>
-        <v>216</v>
+        <v>80</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="5"/>
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="6"/>
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="7"/>
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s">
         <v>120</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>7578</v>
+        <v>5045</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1705,34 +1708,34 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="4"/>
-        <v>85</v>
+        <v>244</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="5"/>
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="6"/>
-        <v>240</v>
+        <v>179</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="7"/>
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
         <v>121</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>6662</v>
+        <v>6913</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1741,34 +1744,34 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="4"/>
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="5"/>
-        <v>34</v>
+        <v>241</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>226</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="7"/>
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="G29" t="s">
         <v>122</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>5262</v>
+        <v>1253</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1777,34 +1780,34 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>225</v>
+        <v>17</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="4"/>
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>244</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="7"/>
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="G30" t="s">
         <v>123</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>1060</v>
+        <v>6611</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,34 +1816,34 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="4"/>
-        <v>223</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="6"/>
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="7"/>
-        <v>250</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
         <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>1334</v>
+        <v>1069</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1849,34 +1852,34 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="4"/>
-        <v>236</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="5"/>
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="6"/>
-        <v>252</v>
+        <v>107</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="7"/>
-        <v>230</v>
+        <v>6</v>
       </c>
       <c r="G32" t="s">
         <v>119</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>6361</v>
+        <v>3570</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1885,34 +1888,34 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="4"/>
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>212</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="6"/>
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="7"/>
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="G33" t="s">
         <v>120</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>4762</v>
+        <v>5246</v>
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,34 +1924,34 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>191</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="4"/>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="6"/>
-        <v>249</v>
+        <v>14</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="7"/>
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
         <v>121</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>1247</v>
+        <v>4215</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1957,34 +1960,34 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="5"/>
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>208</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="7"/>
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="G35" t="s">
         <v>122</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>4617</v>
+        <v>874</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1993,34 +1996,34 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="4"/>
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="6"/>
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="7"/>
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="G36" t="s">
         <v>123</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>2278</v>
+        <v>3539</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2029,34 +2032,34 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>186</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="5"/>
-        <v>51</v>
+        <v>244</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="7"/>
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="G37" t="s">
         <v>1</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>3667</v>
+        <v>7141</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2065,34 +2068,34 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="4"/>
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="5"/>
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="6"/>
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="7"/>
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="G38" t="s">
         <v>119</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>948</v>
+        <v>3419</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2101,34 +2104,34 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="4"/>
-        <v>53</v>
+        <v>204</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="5"/>
-        <v>239</v>
+        <v>13</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="7"/>
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="G39" t="s">
         <v>120</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
-        <v>4994</v>
+        <v>694</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2137,34 +2140,34 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>239</v>
+        <v>158</v>
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="7"/>
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="G40" t="s">
         <v>121</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
-        <v>3342</v>
+        <v>5228</v>
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2173,34 +2176,34 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="5"/>
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="6"/>
-        <v>237</v>
+        <v>180</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="7"/>
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
         <v>122</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>5994</v>
+        <v>7478</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2209,34 +2212,34 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ca="1" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ca="1" si="5"/>
         <v>49</v>
       </c>
-      <c r="C42">
-        <f t="shared" ca="1" si="4"/>
-        <v>66</v>
-      </c>
-      <c r="D42">
-        <f t="shared" ca="1" si="5"/>
-        <v>205</v>
-      </c>
       <c r="E42">
         <f t="shared" ca="1" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ca="1" si="7"/>
         <v>53</v>
-      </c>
-      <c r="F42">
-        <f t="shared" ca="1" si="7"/>
-        <v>251</v>
       </c>
       <c r="G42" t="s">
         <v>123</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>6585</v>
+        <v>2633</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2245,34 +2248,34 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="5"/>
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="6"/>
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="7"/>
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="G43" t="s">
         <v>1</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>3739</v>
+        <v>5318</v>
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2281,34 +2284,34 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>158</v>
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="4"/>
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="5"/>
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="6"/>
-        <v>162</v>
+        <v>8</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="7"/>
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="G44" t="s">
         <v>119</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>604</v>
+        <v>4431</v>
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2317,34 +2320,34 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="4"/>
-        <v>245</v>
+        <v>169</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="5"/>
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="6"/>
-        <v>104</v>
+        <v>242</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="7"/>
-        <v>211</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
         <v>120</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>5875</v>
+        <v>6304</v>
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,34 +2356,34 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>137</v>
+        <v>212</v>
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="4"/>
-        <v>235</v>
+        <v>93</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="5"/>
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="6"/>
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
+        <v>220</v>
       </c>
       <c r="G46" t="s">
         <v>121</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>2079</v>
+        <v>219</v>
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2389,34 +2392,34 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="5"/>
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>179</v>
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="7"/>
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="G47" t="s">
         <v>122</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>2260</v>
+        <v>4071</v>
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2425,34 +2428,34 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="4"/>
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="5"/>
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="6"/>
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="7"/>
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G48" t="s">
         <v>123</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>6979</v>
+        <v>3475</v>
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2461,34 +2464,34 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>111</v>
+        <v>196</v>
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="4"/>
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="5"/>
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="7"/>
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="G49" t="s">
         <v>1</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>4537</v>
+        <v>5442</v>
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,30 +2500,30 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>248</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="5"/>
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="6"/>
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="G50" t="s">
         <v>119</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>259</v>
+        <v>4773</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="3"/>
@@ -2533,34 +2536,34 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="4"/>
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="5"/>
-        <v>159</v>
+        <v>32</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="7"/>
-        <v>122</v>
+        <v>248</v>
       </c>
       <c r="G51" t="s">
         <v>120</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>810</v>
+        <v>3050</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2569,34 +2572,34 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="4"/>
-        <v>231</v>
+        <v>35</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="5"/>
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="6"/>
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="7"/>
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="G52" t="s">
         <v>121</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
-        <v>3157</v>
+        <v>2514</v>
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2605,34 +2608,34 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="5"/>
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="6"/>
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="7"/>
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="G53" t="s">
         <v>122</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>6466</v>
+        <v>1341</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2641,34 +2644,34 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>205</v>
+        <v>72</v>
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>198</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="5"/>
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="6"/>
-        <v>94</v>
+        <v>216</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="7"/>
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="G54" t="s">
         <v>123</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
-        <v>1325</v>
+        <v>1486</v>
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,34 +2680,34 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="4"/>
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="5"/>
-        <v>80</v>
+        <v>194</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="6"/>
-        <v>235</v>
+        <v>2</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="G55" t="s">
         <v>1</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>5381</v>
+        <v>1850</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2717,30 +2720,30 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="4"/>
-        <v>211</v>
+        <v>16</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="5"/>
-        <v>227</v>
+        <v>100</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="6"/>
-        <v>95</v>
+        <v>168</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="7"/>
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G56" t="s">
         <v>119</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>2268</v>
+        <v>7520</v>
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2749,34 +2752,34 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="4"/>
-        <v>190</v>
+        <v>37</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="6"/>
-        <v>115</v>
+        <v>234</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="7"/>
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G57" t="s">
         <v>120</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>3441</v>
+        <v>2912</v>
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2785,34 +2788,34 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="4"/>
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="5"/>
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="7"/>
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="G58" t="s">
         <v>121</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
-        <v>4522</v>
+        <v>2952</v>
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2821,34 +2824,34 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="4"/>
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="5"/>
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="6"/>
-        <v>85</v>
+        <v>218</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="7"/>
-        <v>58</v>
+        <v>247</v>
       </c>
       <c r="G59" t="s">
         <v>122</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>2115</v>
+        <v>1814</v>
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2857,34 +2860,34 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="4"/>
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="5"/>
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="6"/>
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="7"/>
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="G60" t="s">
         <v>123</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
-        <v>181</v>
+        <v>5417</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2893,30 +2896,30 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>193</v>
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="4"/>
-        <v>131</v>
+        <v>254</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="5"/>
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="6"/>
-        <v>228</v>
+        <v>4</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="7"/>
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="G61" t="s">
         <v>1</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>3140</v>
+        <v>4805</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="3"/>
@@ -2929,34 +2932,34 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="4"/>
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="5"/>
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="6"/>
-        <v>243</v>
+        <v>107</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="7"/>
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="G62" t="s">
         <v>119</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>308</v>
+        <v>6324</v>
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2965,34 +2968,34 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="4"/>
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="5"/>
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="7"/>
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="G63" t="s">
         <v>120</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
-        <v>2980</v>
+        <v>3187</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3001,34 +3004,34 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>240</v>
+        <v>93</v>
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="4"/>
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>208</v>
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="6"/>
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="7"/>
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="G64" t="s">
         <v>121</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>4083</v>
+        <v>1010</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3037,34 +3040,34 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="4"/>
-        <v>54</v>
+        <v>244</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="7"/>
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="G65" t="s">
         <v>122</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>5187</v>
+        <v>5211</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3073,34 +3076,34 @@
       </c>
       <c r="B66">
         <f t="shared" ref="B66:B119" ca="1" si="8">RANDBETWEEN(1,255)</f>
-        <v>12</v>
+        <v>204</v>
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="4"/>
-        <v>205</v>
+        <v>74</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="5"/>
-        <v>107</v>
+        <v>220</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="6"/>
-        <v>223</v>
+        <v>48</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="7"/>
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="G66" t="s">
         <v>123</v>
       </c>
       <c r="H66">
         <f t="shared" ref="H66:H119" ca="1" si="9">RANDBETWEEN(1,7800)</f>
-        <v>2539</v>
+        <v>5217</v>
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I119" ca="1" si="10">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3109,34 +3112,34 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="8"/>
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C67">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="5"/>
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="7"/>
-        <v>214</v>
+        <v>24</v>
       </c>
       <c r="G67" t="s">
         <v>1</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="9"/>
-        <v>6209</v>
+        <v>1708</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3145,34 +3148,34 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="8"/>
-        <v>239</v>
+        <v>158</v>
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="4"/>
-        <v>246</v>
+        <v>140</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="5"/>
-        <v>99</v>
+        <v>243</v>
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="6"/>
-        <v>222</v>
+        <v>163</v>
       </c>
       <c r="F68">
         <f t="shared" ca="1" si="7"/>
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="G68" t="s">
         <v>119</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="9"/>
-        <v>6343</v>
+        <v>7033</v>
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3181,34 +3184,34 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="8"/>
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="4"/>
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="5"/>
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="6"/>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="7"/>
-        <v>29</v>
+        <v>200</v>
       </c>
       <c r="G69" t="s">
         <v>120</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="9"/>
-        <v>4903</v>
+        <v>7575</v>
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3217,30 +3220,30 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="8"/>
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="4"/>
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="5"/>
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="7"/>
-        <v>216</v>
+        <v>11</v>
       </c>
       <c r="G70" t="s">
         <v>121</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="9"/>
-        <v>5555</v>
+        <v>6243</v>
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="10"/>
@@ -3253,34 +3256,34 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="8"/>
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="4"/>
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="5"/>
-        <v>210</v>
+        <v>32</v>
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="7"/>
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="G71" t="s">
         <v>122</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="9"/>
-        <v>6879</v>
+        <v>3519</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3289,15 +3292,15 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="8"/>
-        <v>102</v>
+        <v>220</v>
       </c>
       <c r="C72">
         <f t="shared" ca="1" si="4"/>
-        <v>17</v>
+        <v>221</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="5"/>
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="6"/>
@@ -3305,18 +3308,18 @@
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="7"/>
-        <v>135</v>
+        <v>240</v>
       </c>
       <c r="G72" t="s">
         <v>123</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="9"/>
-        <v>2049</v>
+        <v>1924</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3325,34 +3328,34 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="4"/>
-        <v>212</v>
+        <v>163</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="5"/>
-        <v>213</v>
+        <v>254</v>
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="6"/>
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="7"/>
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G73" t="s">
         <v>1</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="9"/>
-        <v>7245</v>
+        <v>3550</v>
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="10"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3361,34 +3364,34 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="8"/>
-        <v>187</v>
+        <v>106</v>
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="4"/>
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="5"/>
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="6"/>
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="7"/>
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="G74" t="s">
         <v>119</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="9"/>
-        <v>6666</v>
+        <v>3493</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3397,34 +3400,34 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="8"/>
-        <v>242</v>
+        <v>97</v>
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="4"/>
-        <v>234</v>
+        <v>171</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="5"/>
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="G75" t="s">
         <v>120</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="9"/>
-        <v>4059</v>
+        <v>4542</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3433,34 +3436,34 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="8"/>
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="7"/>
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="G76" t="s">
         <v>121</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="9"/>
-        <v>4394</v>
+        <v>7187</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3469,34 +3472,34 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="8"/>
-        <v>125</v>
+        <v>232</v>
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="4"/>
-        <v>169</v>
+        <v>106</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="5"/>
-        <v>56</v>
+        <v>162</v>
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="6"/>
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="7"/>
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="G77" t="s">
         <v>122</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="9"/>
-        <v>5973</v>
+        <v>4542</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3505,30 +3508,30 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="8"/>
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="4"/>
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="5"/>
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="6"/>
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="7"/>
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="G78" t="s">
         <v>123</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="9"/>
-        <v>513</v>
+        <v>5987</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="10"/>
@@ -3541,30 +3544,30 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="8"/>
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="4"/>
-        <v>212</v>
+        <v>91</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="5"/>
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="6"/>
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="7"/>
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="G79" t="s">
         <v>1</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="9"/>
-        <v>6582</v>
+        <v>5674</v>
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="10"/>
@@ -3577,34 +3580,34 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="4"/>
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="6"/>
-        <v>151</v>
+        <v>250</v>
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="7"/>
-        <v>56</v>
+        <v>206</v>
       </c>
       <c r="G80" t="s">
         <v>119</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="9"/>
-        <v>2125</v>
+        <v>2290</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3613,34 +3616,34 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="8"/>
-        <v>242</v>
+        <v>6</v>
       </c>
       <c r="C81">
         <f t="shared" ref="C81:C119" ca="1" si="11">RANDBETWEEN(1,255)</f>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D81">
         <f t="shared" ref="D81:D119" ca="1" si="12">RANDBETWEEN(1,255)</f>
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="E81">
         <f t="shared" ref="E81:E119" ca="1" si="13">RANDBETWEEN(1,255)</f>
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="7"/>
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G81" t="s">
         <v>120</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="9"/>
-        <v>4505</v>
+        <v>6388</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,34 +3652,34 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="8"/>
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="11"/>
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="12"/>
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="13"/>
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F82">
         <f t="shared" ref="F82:F119" ca="1" si="14">RANDBETWEEN(1,255)</f>
-        <v>153</v>
+        <v>247</v>
       </c>
       <c r="G82" t="s">
         <v>121</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="9"/>
-        <v>2045</v>
+        <v>7218</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3685,34 +3688,34 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="8"/>
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="11"/>
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="12"/>
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="13"/>
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="14"/>
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="G83" t="s">
         <v>122</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="9"/>
-        <v>6768</v>
+        <v>1652</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3721,34 +3724,34 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="8"/>
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="11"/>
-        <v>216</v>
+        <v>5</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="12"/>
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="13"/>
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="14"/>
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="G84" t="s">
         <v>123</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="9"/>
-        <v>5757</v>
+        <v>3776</v>
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3757,34 +3760,34 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="8"/>
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="11"/>
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="12"/>
-        <v>52</v>
+        <v>171</v>
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="13"/>
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="14"/>
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="G85" t="s">
         <v>1</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="9"/>
-        <v>5319</v>
+        <v>1673</v>
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3793,34 +3796,34 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="8"/>
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="12"/>
-        <v>17</v>
+        <v>247</v>
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="13"/>
-        <v>227</v>
+        <v>12</v>
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="14"/>
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="G86" t="s">
         <v>119</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="9"/>
-        <v>4492</v>
+        <v>1712</v>
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3829,34 +3832,34 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="8"/>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="11"/>
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="12"/>
-        <v>212</v>
+        <v>63</v>
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="13"/>
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="14"/>
-        <v>120</v>
+        <v>18</v>
       </c>
       <c r="G87" t="s">
         <v>120</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="9"/>
-        <v>2971</v>
+        <v>4987</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="10"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3865,34 +3868,34 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="8"/>
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="11"/>
-        <v>220</v>
+        <v>126</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="12"/>
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="13"/>
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="14"/>
-        <v>177</v>
+        <v>118</v>
       </c>
       <c r="G88" t="s">
         <v>121</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="9"/>
-        <v>6166</v>
+        <v>230</v>
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3901,34 +3904,34 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="8"/>
-        <v>25</v>
+        <v>152</v>
       </c>
       <c r="C89">
         <f t="shared" ca="1" si="11"/>
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="12"/>
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="13"/>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="14"/>
-        <v>136</v>
+        <v>229</v>
       </c>
       <c r="G89" t="s">
         <v>122</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="9"/>
-        <v>1064</v>
+        <v>4232</v>
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3937,34 +3940,34 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="8"/>
-        <v>193</v>
+        <v>249</v>
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="11"/>
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="12"/>
-        <v>156</v>
+        <v>201</v>
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="13"/>
-        <v>153</v>
+        <v>235</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="14"/>
-        <v>133</v>
+        <v>185</v>
       </c>
       <c r="G90" t="s">
         <v>123</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="9"/>
-        <v>4573</v>
+        <v>5678</v>
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3973,34 +3976,34 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="8"/>
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="11"/>
-        <v>24</v>
+        <v>221</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="12"/>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="13"/>
-        <v>187</v>
+        <v>110</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="14"/>
-        <v>108</v>
+        <v>245</v>
       </c>
       <c r="G91" t="s">
         <v>1</v>
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="9"/>
-        <v>2495</v>
+        <v>1634</v>
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4009,34 +4012,34 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="8"/>
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="11"/>
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="12"/>
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="13"/>
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="14"/>
-        <v>37</v>
+        <v>217</v>
       </c>
       <c r="G92" t="s">
         <v>119</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="9"/>
-        <v>5495</v>
+        <v>3724</v>
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4045,34 +4048,34 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="8"/>
-        <v>130</v>
+        <v>199</v>
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="11"/>
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="12"/>
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="13"/>
-        <v>233</v>
+        <v>10</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="14"/>
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="G93" t="s">
         <v>120</v>
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="9"/>
-        <v>2941</v>
+        <v>4005</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4081,34 +4084,34 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="8"/>
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="11"/>
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="12"/>
-        <v>187</v>
+        <v>84</v>
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="13"/>
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="14"/>
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G94" t="s">
         <v>121</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="9"/>
-        <v>316</v>
+        <v>2709</v>
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4117,34 +4120,34 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="8"/>
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="11"/>
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="12"/>
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="13"/>
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="14"/>
-        <v>254</v>
+        <v>12</v>
       </c>
       <c r="G95" t="s">
         <v>122</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="9"/>
-        <v>6008</v>
+        <v>5838</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4153,34 +4156,34 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="11"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="12"/>
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="13"/>
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="14"/>
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="G96" t="s">
         <v>123</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="9"/>
-        <v>2805</v>
+        <v>2494</v>
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4189,34 +4192,34 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="11"/>
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="12"/>
-        <v>222</v>
+        <v>130</v>
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="13"/>
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="14"/>
-        <v>236</v>
+        <v>152</v>
       </c>
       <c r="G97" t="s">
         <v>1</v>
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="9"/>
-        <v>1826</v>
+        <v>7591</v>
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4225,34 +4228,34 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="8"/>
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="11"/>
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="12"/>
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="13"/>
-        <v>214</v>
+        <v>86</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="14"/>
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="G98" t="s">
         <v>119</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="9"/>
-        <v>1344</v>
+        <v>3116</v>
       </c>
       <c r="I98">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4261,34 +4264,34 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="8"/>
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="11"/>
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="12"/>
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="13"/>
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="14"/>
-        <v>13</v>
+        <v>242</v>
       </c>
       <c r="G99" t="s">
         <v>120</v>
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="9"/>
-        <v>3919</v>
+        <v>2726</v>
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4297,34 +4300,34 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="8"/>
-        <v>219</v>
+        <v>88</v>
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="11"/>
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="12"/>
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="13"/>
-        <v>151</v>
+        <v>226</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="14"/>
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="G100" t="s">
         <v>121</v>
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="9"/>
-        <v>570</v>
+        <v>4861</v>
       </c>
       <c r="I100">
         <f t="shared" ca="1" si="10"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4333,34 +4336,34 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="8"/>
-        <v>243</v>
+        <v>7</v>
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="11"/>
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="12"/>
-        <v>239</v>
+        <v>112</v>
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="13"/>
-        <v>20</v>
+        <v>192</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="14"/>
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="G101" t="s">
         <v>122</v>
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="9"/>
-        <v>3731</v>
+        <v>4583</v>
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="10"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4369,34 +4372,34 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="8"/>
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="C102">
         <f t="shared" ca="1" si="11"/>
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="12"/>
-        <v>220</v>
+        <v>129</v>
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="13"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="14"/>
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="G102" t="s">
         <v>123</v>
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="9"/>
-        <v>7572</v>
+        <v>1147</v>
       </c>
       <c r="I102">
         <f t="shared" ca="1" si="10"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4405,34 +4408,34 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="8"/>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C103">
         <f t="shared" ca="1" si="11"/>
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="12"/>
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E103">
         <f t="shared" ca="1" si="13"/>
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="F103">
         <f t="shared" ca="1" si="14"/>
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="G103" t="s">
         <v>1</v>
       </c>
       <c r="H103">
         <f t="shared" ca="1" si="9"/>
-        <v>741</v>
+        <v>5910</v>
       </c>
       <c r="I103">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4441,30 +4444,30 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="11"/>
-        <v>207</v>
+        <v>238</v>
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="12"/>
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="E104">
         <f t="shared" ca="1" si="13"/>
-        <v>234</v>
+        <v>99</v>
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="14"/>
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="G104" t="s">
         <v>119</v>
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="9"/>
-        <v>7764</v>
+        <v>4075</v>
       </c>
       <c r="I104">
         <f t="shared" ca="1" si="10"/>
@@ -4477,34 +4480,34 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="8"/>
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="C105">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="12"/>
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E105">
         <f t="shared" ca="1" si="13"/>
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="14"/>
-        <v>238</v>
+        <v>5</v>
       </c>
       <c r="G105" t="s">
         <v>120</v>
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="9"/>
-        <v>4000</v>
+        <v>585</v>
       </c>
       <c r="I105">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4513,34 +4516,34 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="8"/>
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="C106">
         <f t="shared" ca="1" si="11"/>
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="12"/>
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="E106">
         <f t="shared" ca="1" si="13"/>
-        <v>216</v>
+        <v>20</v>
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="14"/>
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="G106" t="s">
         <v>121</v>
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="9"/>
-        <v>4017</v>
+        <v>5806</v>
       </c>
       <c r="I106">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4549,34 +4552,34 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="8"/>
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="C107">
         <f t="shared" ca="1" si="11"/>
-        <v>36</v>
+        <v>154</v>
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="12"/>
-        <v>229</v>
+        <v>8</v>
       </c>
       <c r="E107">
         <f t="shared" ca="1" si="13"/>
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="14"/>
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="G107" t="s">
         <v>122</v>
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="9"/>
-        <v>945</v>
+        <v>993</v>
       </c>
       <c r="I107">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4585,66 +4588,66 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="8"/>
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="C108">
         <f t="shared" ca="1" si="11"/>
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="12"/>
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="E108">
         <f t="shared" ca="1" si="13"/>
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="F108">
         <f t="shared" ca="1" si="14"/>
-        <v>252</v>
+        <v>107</v>
       </c>
       <c r="G108" t="s">
         <v>123</v>
       </c>
       <c r="H108">
         <f t="shared" ca="1" si="9"/>
-        <v>4540</v>
+        <v>1457</v>
       </c>
       <c r="I108">
         <f t="shared" ca="1" si="10"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="8"/>
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="C109">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>251</v>
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="12"/>
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E109">
         <f t="shared" ca="1" si="13"/>
-        <v>193</v>
+        <v>120</v>
       </c>
       <c r="F109">
         <f t="shared" ca="1" si="14"/>
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="G109" t="s">
         <v>1</v>
       </c>
       <c r="H109">
         <f t="shared" ca="1" si="9"/>
-        <v>3925</v>
+        <v>334</v>
       </c>
       <c r="I109">
         <f t="shared" ca="1" si="10"/>
@@ -4657,34 +4660,34 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="8"/>
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="C110">
         <f t="shared" ca="1" si="11"/>
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="12"/>
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="E110">
         <f t="shared" ca="1" si="13"/>
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="F110">
         <f t="shared" ca="1" si="14"/>
-        <v>238</v>
+        <v>88</v>
       </c>
       <c r="G110" t="s">
         <v>119</v>
       </c>
       <c r="H110">
         <f t="shared" ca="1" si="9"/>
-        <v>1229</v>
+        <v>1812</v>
       </c>
       <c r="I110">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4693,34 +4696,34 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="8"/>
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C111">
         <f t="shared" ca="1" si="11"/>
-        <v>44</v>
+        <v>200</v>
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="12"/>
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E111">
         <f t="shared" ca="1" si="13"/>
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F111">
         <f t="shared" ca="1" si="14"/>
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G111" t="s">
         <v>120</v>
       </c>
       <c r="H111">
         <f t="shared" ca="1" si="9"/>
-        <v>6878</v>
+        <v>6810</v>
       </c>
       <c r="I111">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4729,34 +4732,34 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="8"/>
-        <v>250</v>
+        <v>197</v>
       </c>
       <c r="C112">
         <f t="shared" ca="1" si="11"/>
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="12"/>
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="E112">
         <f t="shared" ca="1" si="13"/>
-        <v>233</v>
+        <v>187</v>
       </c>
       <c r="F112">
         <f t="shared" ca="1" si="14"/>
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="G112" t="s">
         <v>121</v>
       </c>
       <c r="H112">
         <f t="shared" ca="1" si="9"/>
-        <v>1183</v>
+        <v>3636</v>
       </c>
       <c r="I112">
         <f t="shared" ca="1" si="10"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4765,34 +4768,34 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="8"/>
-        <v>226</v>
+        <v>5</v>
       </c>
       <c r="C113">
         <f t="shared" ca="1" si="11"/>
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="D113">
         <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="E113">
         <f t="shared" ca="1" si="13"/>
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="F113">
         <f t="shared" ca="1" si="14"/>
-        <v>206</v>
+        <v>94</v>
       </c>
       <c r="G113" t="s">
         <v>122</v>
       </c>
       <c r="H113">
         <f t="shared" ca="1" si="9"/>
-        <v>7541</v>
+        <v>100</v>
       </c>
       <c r="I113">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4801,30 +4804,30 @@
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="8"/>
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="C114">
         <f t="shared" ca="1" si="11"/>
-        <v>111</v>
+        <v>218</v>
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="12"/>
-        <v>167</v>
+        <v>86</v>
       </c>
       <c r="E114">
         <f t="shared" ca="1" si="13"/>
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="F114">
         <f t="shared" ca="1" si="14"/>
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G114" t="s">
         <v>123</v>
       </c>
       <c r="H114">
         <f t="shared" ca="1" si="9"/>
-        <v>2086</v>
+        <v>440</v>
       </c>
       <c r="I114">
         <f t="shared" ca="1" si="10"/>
@@ -4837,34 +4840,34 @@
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="8"/>
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C115">
         <f t="shared" ca="1" si="11"/>
-        <v>182</v>
+        <v>91</v>
       </c>
       <c r="D115">
         <f t="shared" ca="1" si="12"/>
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="E115">
         <f t="shared" ca="1" si="13"/>
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="F115">
         <f t="shared" ca="1" si="14"/>
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="G115" t="s">
         <v>1</v>
       </c>
       <c r="H115">
         <f t="shared" ca="1" si="9"/>
-        <v>6524</v>
+        <v>7426</v>
       </c>
       <c r="I115">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4873,34 +4876,34 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="8"/>
-        <v>139</v>
+        <v>254</v>
       </c>
       <c r="C116">
         <f t="shared" ca="1" si="11"/>
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="D116">
         <f t="shared" ca="1" si="12"/>
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="E116">
         <f t="shared" ca="1" si="13"/>
-        <v>215</v>
+        <v>145</v>
       </c>
       <c r="F116">
         <f t="shared" ca="1" si="14"/>
-        <v>247</v>
+        <v>115</v>
       </c>
       <c r="G116" t="s">
         <v>119</v>
       </c>
       <c r="H116">
         <f t="shared" ca="1" si="9"/>
-        <v>3150</v>
+        <v>5479</v>
       </c>
       <c r="I116">
         <f t="shared" ca="1" si="10"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4909,34 +4912,34 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="8"/>
-        <v>219</v>
+        <v>25</v>
       </c>
       <c r="C117">
         <f t="shared" ca="1" si="11"/>
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D117">
         <f t="shared" ca="1" si="12"/>
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="E117">
         <f t="shared" ca="1" si="13"/>
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="F117">
         <f t="shared" ca="1" si="14"/>
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="G117" t="s">
         <v>120</v>
       </c>
       <c r="H117">
         <f t="shared" ca="1" si="9"/>
-        <v>5166</v>
+        <v>1161</v>
       </c>
       <c r="I117">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4945,34 +4948,34 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="8"/>
-        <v>242</v>
+        <v>103</v>
       </c>
       <c r="C118">
         <f t="shared" ca="1" si="11"/>
-        <v>157</v>
+        <v>237</v>
       </c>
       <c r="D118">
         <f t="shared" ca="1" si="12"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E118">
         <f t="shared" ca="1" si="13"/>
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="F118">
         <f t="shared" ca="1" si="14"/>
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G118" t="s">
         <v>121</v>
       </c>
       <c r="H118">
         <f t="shared" ca="1" si="9"/>
-        <v>3923</v>
+        <v>3560</v>
       </c>
       <c r="I118">
         <f t="shared" ca="1" si="10"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4981,34 +4984,34 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="8"/>
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="C119">
         <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="D119">
         <f t="shared" ca="1" si="12"/>
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E119">
         <f t="shared" ca="1" si="13"/>
-        <v>227</v>
+        <v>160</v>
       </c>
       <c r="F119">
         <f t="shared" ca="1" si="14"/>
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G119" t="s">
         <v>122</v>
       </c>
       <c r="H119">
         <f t="shared" ca="1" si="9"/>
-        <v>661</v>
+        <v>6133</v>
       </c>
       <c r="I119">
         <f t="shared" ca="1" si="10"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>